<commit_message>
Added existing dialogues for chapter 1
</commit_message>
<xml_diff>
--- a/src/Cyberpunk2078/Assets/Xlsx/Text.xlsx
+++ b/src/Cyberpunk2078/Assets/Xlsx/Text.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1853B5B-9C50-439A-A9D1-1B4A03344294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73087A8-6050-4508-9522-4FCB21C6FBFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11085" yWindow="1830" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,71 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{0E234BC9-8F17-4963-BD92-92D3511137A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+10000+Index</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{63EFA572-4E41-41A4-9A4C-DD7C14C5BEB0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Zheyu Zhang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+1    01     01    01   001
+1 Chapter Level Scene Index</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Game Start</t>
   </si>
@@ -46,6 +109,158 @@
   </si>
   <si>
     <t>english</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hey, Lyu! Did you get the target information?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I think so, give me some time to check.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>It seems like you need to drop a harder lesson.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>We are bounty hunters. They pay, we kill.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>You know, this dumb virtual world where you are living is ruleless</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aight... Aight...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>It has been a while since the last workout. Let's see if you are rusty.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The floor under your feet seems vulnerable. Break it!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oh, a gate. The control trigger should be somewhere around.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BY YOU!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I have been forced to log out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TWICE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>There will be no third time. In this distance, you are so dead.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What was that?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What happened?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I reflected a bullet.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Are you joking?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>It was real, Todd.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Just focus on the mission, Lyu. It was weird and we need to figure that out later.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I am sure it was not a phantom or poisoned symptom. I just can feel a deeper connection with everything.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I found some weird floating orbs in the air. Any idea about what they are?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weird floating orbs? Are they in blue color?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wait... It can't be...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A girl?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oh, they are still chasing. I'd better hurry.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lyu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Todd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jack, male...</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wait... Jack again? Is this the third mission on this guy we got this month?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>You... You... You again?! The goddamn "E-Ghost"!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Those orbs are data interpreters of this virtual world. They should not be seen by a human client. They would give you extra momentum for doing more staff.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>An emergency exit is located on the top of this building. I did not find any drones or guards nearby.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>It is weird. Why do those guards and drones keep chasing me? Jack was already forced to sign out and they are supposed to stop functioning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Go across the dancing bar. The exit should be able to get you safely out of there.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -53,7 +268,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +290,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -90,7 +320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -98,13 +328,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -384,17 +647,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.75" customWidth="1"/>
-    <col min="2" max="2" width="38.125" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -453,9 +717,330 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>10000</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>10001</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10002</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10003</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>1010101001</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>1010101002</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>1010101003</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>1010101004</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>1010101005</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>1010101006</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>1010101007</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>1010101008</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>1010101009</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>1010101010</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>1010102001</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>1010103001</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>1010104001</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>1010104002</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>1010104003</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>1010104004</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>1010104005</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>1010104006</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>1010104007</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>1010104008</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>1010104009</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>1010104010</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>1010104011</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>1010104012</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>1010104013</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>1010105001</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>1010105002</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>1010105003</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>1010105004</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>1010105005</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>1010105006</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1010201001</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1010201002</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1010201003</v>
+      </c>
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>1010301001</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>1010301002</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wrap up Semaster 1
</commit_message>
<xml_diff>
--- a/src/Cyberpunk2078/Assets/Xlsx/Text.xlsx
+++ b/src/Cyberpunk2078/Assets/Xlsx/Text.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE098FBB-4334-4ED9-A12B-67F5C309A780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367EEE2E-6C29-4BA3-9585-8F41D3F83385}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="7710" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Game Start</t>
   </si>
@@ -132,10 +132,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Aight... Aight...</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>It has been a while since the last workout. Let's see if you are rusty.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -144,10 +140,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Oh, a gate. The control trigger should be somewhere around.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BY YOU!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -168,14 +160,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>I reflected a bullet.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Are you joking?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>It was real, Todd.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -184,14 +168,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Just focus on the mission, Lyu. It was weird and we need to figure that out later.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I am sure it was not a phantom or poisoned symptom. I just can feel a deeper connection with everything.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>I found some weird floating orbs in the air. Any idea about what they are?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -269,6 +245,34 @@
   </si>
   <si>
     <t>???</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alright…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I deflected a bullet.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I am sure it was not a illusion. I just can feel a deeper connection with everything.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is everything ok?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hah, you must be kidding.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Just focus on the mission, Lyu. It was weird and we will figure that out later.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Search around. The key should be nearby.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -276,7 +280,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,18 +663,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.9"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="60.625" customWidth="1"/>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="60.59765625" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -678,7 +682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -686,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -694,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -702,7 +706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -710,7 +714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -718,7 +722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -726,47 +730,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>10000</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>10001</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>10002</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>10003</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>10004</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="2" customFormat="1">
       <c r="A13" s="2">
         <v>1010101001</v>
       </c>
@@ -774,7 +778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" s="3" customFormat="1">
       <c r="A14" s="3">
         <v>1010101002</v>
       </c>
@@ -782,23 +786,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" s="3" customFormat="1">
       <c r="A15" s="3">
         <v>1010101003</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="3" customFormat="1">
       <c r="A16" s="3">
         <v>1010101004</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="3" customFormat="1">
       <c r="A17" s="3">
         <v>1010101005</v>
       </c>
@@ -806,15 +810,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" s="3" customFormat="1">
       <c r="A18" s="3">
         <v>1010101006</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="3" customFormat="1">
       <c r="A19" s="3">
         <v>1010101007</v>
       </c>
@@ -822,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" s="3" customFormat="1">
       <c r="A20" s="3">
         <v>1010101008</v>
       </c>
@@ -830,244 +834,244 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" s="3" customFormat="1">
       <c r="A21" s="3">
         <v>1010101009</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="4" customFormat="1">
       <c r="A22" s="4">
         <v>1010101010</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="5" customFormat="1">
       <c r="A23" s="5">
         <v>1010102001</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="5" customFormat="1">
       <c r="A24" s="5">
         <v>1010103001</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1">
       <c r="A25" s="2">
         <v>1010104001</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="3" customFormat="1">
       <c r="A26" s="3">
         <v>1010104002</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="3" customFormat="1">
       <c r="A27" s="3">
         <v>1010104003</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="3" customFormat="1">
       <c r="A28" s="3">
         <v>1010104004</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="3" customFormat="1">
       <c r="A29" s="3">
         <v>1010104005</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="4" customFormat="1">
       <c r="A30" s="4">
         <v>1010104006</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1">
       <c r="A31" s="2">
         <v>1010105001</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="3" customFormat="1">
       <c r="A32" s="3">
         <v>1010105002</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="3" customFormat="1">
       <c r="A33" s="3">
         <v>1010105003</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="3" customFormat="1">
       <c r="A34" s="3">
         <v>1010105004</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="3" customFormat="1">
       <c r="A35" s="3">
         <v>1010105005</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="3" customFormat="1">
       <c r="A36" s="6">
         <v>1010105006</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="2" customFormat="1">
       <c r="A37" s="2">
         <v>1010106001</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="3" customFormat="1">
       <c r="A38" s="3">
         <v>1010106002</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="3" customFormat="1">
       <c r="A39" s="3">
         <v>1010106003</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="3" customFormat="1">
       <c r="A40" s="3">
         <v>1010106004</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="3" customFormat="1">
       <c r="A41" s="3">
         <v>1010106005</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="3" customFormat="1">
       <c r="A42" s="3">
         <v>1010106006</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="3" customFormat="1">
       <c r="A43" s="3">
         <v>1010106007</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="4" customFormat="1">
       <c r="A44" s="4">
         <v>1010106008</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>1010201001</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>1010201002</v>
       </c>
       <c r="B46" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>1010201003</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>1010201004</v>
       </c>
       <c r="B48" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="2" customFormat="1">
       <c r="A49" s="2">
         <v>1010301001</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="4" customFormat="1">
       <c r="A50" s="4">
         <v>1010301002</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>